<commit_message>
Added a few notes about 2018, 2019 lineups
</commit_message>
<xml_diff>
--- a/positional data.xlsx
+++ b/positional data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MEGA\MEGAsync Uploads\Y2 Project\2021-UoA-DATASCI-792-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEC253BD-2E76-4539-AA62-AA11929F35AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD2B5C1-B803-4ADF-ABB6-A95EB7951304}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6585" yWindow="285" windowWidth="21600" windowHeight="13530"/>
+    <workbookView xWindow="8745" yWindow="375" windowWidth="21600" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positional data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -278,13 +278,37 @@
   </si>
   <si>
     <t>2018 Wk7 vs Otago - Joe Ravouvou named at 23</t>
+  </si>
+  <si>
+    <t>2019 Wk1 vs North Harbour - Kurt Heatherley named at 23</t>
+  </si>
+  <si>
+    <t>2019 Wk2, 3, 4 vs Northland, BOP, Waikato - Peter-Chanel Tagaloa named at 19, Kurt Heatherley named at 23</t>
+  </si>
+  <si>
+    <t>2019 Wk5 vs Canterbury - Peter-Chanel Tagaloa named at 4</t>
+  </si>
+  <si>
+    <t>2019 Wk5 vs Canterbury - Kurt Heatherley named at 15</t>
+  </si>
+  <si>
+    <t>2019 Wk6 vs Counties Manukau - Peter-Chanel Tagaloa named at 4</t>
+  </si>
+  <si>
+    <t>2019 Wk6 vs Counties Manukau - Kurt Heatherley named at 15</t>
+  </si>
+  <si>
+    <t>2019 Wk6 vs Counties Manukau - Cameron Suafoa named at 6</t>
+  </si>
+  <si>
+    <t>2019 Wk10 vs Taranaki - Kurt Heatherley named at 23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +439,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1118,11 +1148,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:R67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="Q76" sqref="Q76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1760,42 @@
         <v>85</v>
       </c>
     </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q71" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>88</v>
+      </c>
+      <c r="P73" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>90</v>
+      </c>
+      <c r="G74" t="s">
+        <v>92</v>
+      </c>
+      <c r="P74" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q75" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed most of the positional data
Still a few blanks and some clarifications needed from Paul, will hopefully get some info from him via email
</commit_message>
<xml_diff>
--- a/positional data.xlsx
+++ b/positional data.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MEGA\MEGAsync Uploads\Y2 Project\2021-UoA-DATASCI-792-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD2B5C1-B803-4ADF-ABB6-A95EB7951304}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42168F24-783B-4FDE-8E2D-E76491CE76F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="375" windowWidth="21600" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6585" yWindow="285" windowWidth="21600" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positional data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -302,6 +313,69 @@
   </si>
   <si>
     <t>2019 Wk10 vs Taranaki - Kurt Heatherley named at 23</t>
+  </si>
+  <si>
+    <t>Pref. group</t>
+  </si>
+  <si>
+    <t>Front row</t>
+  </si>
+  <si>
+    <t>Flanker</t>
+  </si>
+  <si>
+    <t>Prop</t>
+  </si>
+  <si>
+    <t>Hooker</t>
+  </si>
+  <si>
+    <t>Preferred group based on preferred position</t>
+  </si>
+  <si>
+    <t>Pref. pos. (text)</t>
+  </si>
+  <si>
+    <t>Pref. pos. (number)</t>
+  </si>
+  <si>
+    <t>Preferred position (number) based on most selections</t>
+  </si>
+  <si>
+    <t>Back row</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>Outside backs</t>
+  </si>
+  <si>
+    <t>Preferred position (text) based on preferred position (number); is a generic descriptor (i.e. loosehead and tighthead props are just classified as "prop"), since number will differentiate between the two</t>
+  </si>
+  <si>
+    <t>Number 8</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>Players with only replacement selections have their preferred positions/groups selected through 1) looking for information online 2) observing substitutions in their appearances</t>
+  </si>
+  <si>
+    <t>Centre</t>
+  </si>
+  <si>
+    <t>Inside backs</t>
+  </si>
+  <si>
+    <t>Scrum-half</t>
+  </si>
+  <si>
+    <t>Fly-half</t>
+  </si>
+  <si>
+    <t>Fullback</t>
   </si>
 </sst>
 </file>
@@ -1149,15 +1223,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="Q76" sqref="Q76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1210,488 +1284,4028 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>22</v>
+      </c>
+      <c r="R3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" t="s">
+        <v>97</v>
+      </c>
+      <c r="T3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>98</v>
+      </c>
+      <c r="T4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
       <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>7</v>
+      </c>
+      <c r="S5" t="s">
+        <v>96</v>
+      </c>
+      <c r="T5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
       <c r="O6">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
       </c>
       <c r="Q6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>14</v>
+      </c>
+      <c r="S6" t="s">
+        <v>104</v>
+      </c>
+      <c r="T6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>14</v>
+      </c>
+      <c r="S7" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>8</v>
+      </c>
+      <c r="S8" t="s">
+        <v>107</v>
+      </c>
+      <c r="T8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="S9" t="s">
+        <v>108</v>
+      </c>
+      <c r="T9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
       <c r="Q10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10" t="s">
+        <v>108</v>
+      </c>
+      <c r="T10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
       <c r="M12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>12</v>
+      </c>
+      <c r="S12" t="s">
+        <v>110</v>
+      </c>
+      <c r="T12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>5</v>
+      </c>
+      <c r="S13" t="s">
+        <v>108</v>
+      </c>
+      <c r="T13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
       </c>
       <c r="Q14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="R14">
+        <v>3</v>
+      </c>
+      <c r="S14" t="s">
+        <v>97</v>
+      </c>
+      <c r="T14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>12</v>
+      </c>
+      <c r="S15" t="s">
+        <v>110</v>
+      </c>
+      <c r="T15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
       <c r="J16">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
       </c>
       <c r="Q16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R16">
+        <v>9</v>
+      </c>
+      <c r="S16" t="s">
+        <v>112</v>
+      </c>
+      <c r="T16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>9</v>
+      </c>
+      <c r="S17" t="s">
+        <v>112</v>
+      </c>
+      <c r="T17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
       <c r="H18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>7</v>
+      </c>
+      <c r="S18" t="s">
+        <v>96</v>
+      </c>
+      <c r="T18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <v>5</v>
+      </c>
+      <c r="S19" t="s">
+        <v>108</v>
+      </c>
+      <c r="T19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>8</v>
+      </c>
+      <c r="R20">
+        <v>10</v>
+      </c>
+      <c r="S20" t="s">
+        <v>113</v>
+      </c>
+      <c r="T20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21" t="s">
+        <v>97</v>
+      </c>
+      <c r="T21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
       <c r="I22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <v>8</v>
+      </c>
+      <c r="S22" t="s">
+        <v>107</v>
+      </c>
+      <c r="T22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>13</v>
+      </c>
+      <c r="S23" t="s">
+        <v>110</v>
+      </c>
+      <c r="T23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>5</v>
+      </c>
+      <c r="R24">
+        <v>7</v>
+      </c>
+      <c r="S24" t="s">
+        <v>96</v>
+      </c>
+      <c r="T24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>4</v>
+      </c>
+      <c r="S25" t="s">
+        <v>108</v>
+      </c>
+      <c r="T25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
       <c r="Q26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="R26">
+        <v>10</v>
+      </c>
+      <c r="S26" t="s">
+        <v>113</v>
+      </c>
+      <c r="T26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
       <c r="Q27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R27">
+        <v>3</v>
+      </c>
+      <c r="S27" t="s">
+        <v>97</v>
+      </c>
+      <c r="T27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>15</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>14</v>
+      </c>
+      <c r="S28" t="s">
+        <v>104</v>
+      </c>
+      <c r="T28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>45</v>
       </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
       <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
         <v>1</v>
       </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
       <c r="Q29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="R29">
+        <v>4</v>
+      </c>
+      <c r="S29" t="s">
+        <v>108</v>
+      </c>
+      <c r="T29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>3</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30" t="s">
+        <v>97</v>
+      </c>
+      <c r="T30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <v>2</v>
+      </c>
+      <c r="S31" t="s">
+        <v>98</v>
+      </c>
+      <c r="T31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
       <c r="E32">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
       </c>
       <c r="Q32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>4</v>
+      </c>
+      <c r="S32" t="s">
+        <v>108</v>
+      </c>
+      <c r="T32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>3</v>
+      </c>
+      <c r="R33">
+        <v>10</v>
+      </c>
+      <c r="S33" t="s">
+        <v>113</v>
+      </c>
+      <c r="T33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>2</v>
+      </c>
+      <c r="R34">
+        <v>9</v>
+      </c>
+      <c r="S34" t="s">
+        <v>112</v>
+      </c>
+      <c r="T34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
       <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>6</v>
+      </c>
+      <c r="R35">
         <v>1</v>
       </c>
-      <c r="Q35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S35" t="s">
+        <v>97</v>
+      </c>
+      <c r="T35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
       <c r="N36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+      <c r="R36">
+        <v>13</v>
+      </c>
+      <c r="S36" t="s">
+        <v>110</v>
+      </c>
+      <c r="T36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>53</v>
       </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
       <c r="O37">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>14</v>
+      </c>
+      <c r="S37" t="s">
+        <v>104</v>
+      </c>
+      <c r="T37" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>54</v>
       </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
       <c r="E38">
         <v>1</v>
       </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
       <c r="G38">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
       </c>
       <c r="Q38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="R38">
+        <v>6</v>
+      </c>
+      <c r="S38" t="s">
+        <v>96</v>
+      </c>
+      <c r="T38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39" t="s">
+        <v>97</v>
+      </c>
+      <c r="T39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>56</v>
       </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
       <c r="G40">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
       </c>
       <c r="Q40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="R40">
+        <v>6</v>
+      </c>
+      <c r="S40" t="s">
+        <v>96</v>
+      </c>
+      <c r="T40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>6</v>
+      </c>
+      <c r="S41" t="s">
+        <v>96</v>
+      </c>
+      <c r="T41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
       <c r="K42">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <v>2</v>
+      </c>
+      <c r="R42">
+        <v>10</v>
+      </c>
+      <c r="S42" t="s">
+        <v>113</v>
+      </c>
+      <c r="T42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>59</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <v>0</v>
       </c>
       <c r="Q43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="S43" t="s">
+        <v>97</v>
+      </c>
+      <c r="T43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>60</v>
       </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
       <c r="L44">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>4</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>11</v>
+      </c>
+      <c r="S44" t="s">
+        <v>104</v>
+      </c>
+      <c r="T44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>61</v>
       </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>5</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>7</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
       <c r="Q45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="R45">
+        <v>8</v>
+      </c>
+      <c r="S45" t="s">
+        <v>107</v>
+      </c>
+      <c r="T45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>62</v>
       </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
       <c r="D46">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>5</v>
+      </c>
+      <c r="R46">
+        <v>3</v>
+      </c>
+      <c r="S46" t="s">
+        <v>97</v>
+      </c>
+      <c r="T46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="R47">
+        <v>2</v>
+      </c>
+      <c r="S47" t="s">
+        <v>98</v>
+      </c>
+      <c r="T47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>64</v>
       </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
       <c r="J48">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
       </c>
       <c r="Q48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="R48">
+        <v>9</v>
+      </c>
+      <c r="S48" t="s">
+        <v>112</v>
+      </c>
+      <c r="T48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>65</v>
       </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
       <c r="Q49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>2</v>
+      </c>
+      <c r="S49" t="s">
+        <v>98</v>
+      </c>
+      <c r="T49" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>13</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>4</v>
+      </c>
+      <c r="S50" t="s">
+        <v>108</v>
+      </c>
+      <c r="T50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>2</v>
+      </c>
+      <c r="S51" t="s">
+        <v>108</v>
+      </c>
+      <c r="T51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>68</v>
       </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
       <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>18</v>
+      </c>
+      <c r="R52">
         <v>2</v>
       </c>
-      <c r="Q52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S52" t="s">
+        <v>98</v>
+      </c>
+      <c r="T52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>69</v>
       </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
       <c r="G53">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>7</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
       </c>
       <c r="Q53">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="R53">
+        <v>8</v>
+      </c>
+      <c r="S53" t="s">
+        <v>107</v>
+      </c>
+      <c r="T53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>7</v>
+      </c>
+      <c r="Q54">
+        <v>3</v>
+      </c>
+      <c r="R54">
+        <v>15</v>
+      </c>
+      <c r="S54" t="s">
+        <v>114</v>
+      </c>
+      <c r="T54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>2</v>
+      </c>
+      <c r="R55">
+        <v>3</v>
+      </c>
+      <c r="S55" t="s">
+        <v>97</v>
+      </c>
+      <c r="T55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>2</v>
+      </c>
+      <c r="S56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>73</v>
       </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
       <c r="M57">
+        <v>4</v>
+      </c>
+      <c r="N57">
+        <v>6</v>
+      </c>
+      <c r="O57">
         <v>1</v>
       </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
       <c r="Q57">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="R57">
+        <v>13</v>
+      </c>
+      <c r="S57" t="s">
+        <v>110</v>
+      </c>
+      <c r="T57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>74</v>
       </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
       <c r="P58">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="Q58">
+        <v>3</v>
+      </c>
+      <c r="R58">
+        <v>15</v>
+      </c>
+      <c r="S58" t="s">
+        <v>114</v>
+      </c>
+      <c r="T58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>2</v>
+      </c>
+      <c r="R59">
+        <v>6</v>
+      </c>
+      <c r="S59" t="s">
+        <v>96</v>
+      </c>
+      <c r="T59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>76</v>
       </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
       <c r="E60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+      <c r="R60">
+        <v>4</v>
+      </c>
+      <c r="S60" t="s">
+        <v>108</v>
+      </c>
+      <c r="T60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>4</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>3</v>
+      </c>
+      <c r="R61">
+        <v>8</v>
+      </c>
+      <c r="S61" t="s">
+        <v>107</v>
+      </c>
+      <c r="T61" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <v>16</v>
+      </c>
+      <c r="R62">
+        <v>9</v>
+      </c>
+      <c r="S62" t="s">
+        <v>112</v>
+      </c>
+      <c r="T62" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <v>3</v>
+      </c>
+      <c r="S63" t="s">
+        <v>97</v>
+      </c>
+      <c r="T63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>80</v>
       </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>0</v>
+      </c>
       <c r="P64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q64">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="R64">
+        <v>15</v>
+      </c>
+      <c r="S64" t="s">
+        <v>114</v>
+      </c>
+      <c r="T64" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>2</v>
+      </c>
+      <c r="R65">
+        <v>2</v>
+      </c>
+      <c r="S65" t="s">
+        <v>98</v>
+      </c>
+      <c r="T65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>82</v>
       </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
       <c r="F66">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <v>5</v>
+      </c>
+      <c r="S66" t="s">
+        <v>108</v>
+      </c>
+      <c r="T66" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -1746,8 +5360,11 @@
       <c r="R67" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S67" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H69" t="s">
         <v>83</v>
       </c>
@@ -1755,22 +5372,22 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q70" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q71" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q72" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
         <v>88</v>
       </c>
@@ -1778,7 +5395,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
         <v>90</v>
       </c>
@@ -1789,9 +5406,29 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q75" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed clarifications from email with Paul
As far as I'm concerned, the positional data is pretty much done
</commit_message>
<xml_diff>
--- a/positional data.xlsx
+++ b/positional data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MEGA\MEGAsync Uploads\Y2 Project\2021-UoA-DATASCI-792-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42168F24-783B-4FDE-8E2D-E76491CE76F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E0E031-A629-478E-9712-D883497980C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6585" yWindow="285" windowWidth="21600" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="3945" windowWidth="21600" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positional data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:T81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1903,6 +1903,15 @@
       <c r="Q11">
         <v>0</v>
       </c>
+      <c r="R11">
+        <v>8</v>
+      </c>
+      <c r="S11" t="s">
+        <v>107</v>
+      </c>
+      <c r="T11" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -4374,8 +4383,11 @@
       <c r="Q51">
         <v>2</v>
       </c>
+      <c r="R51">
+        <v>6</v>
+      </c>
       <c r="S51" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="T51" t="s">
         <v>103</v>
@@ -4681,8 +4693,14 @@
       <c r="Q56">
         <v>2</v>
       </c>
+      <c r="R56">
+        <v>12</v>
+      </c>
       <c r="S56" t="s">
         <v>110</v>
+      </c>
+      <c r="T56" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed some column names on the bottom
now it's DEFINITELY done
</commit_message>
<xml_diff>
--- a/positional data.xlsx
+++ b/positional data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MEGA\MEGAsync Uploads\Y2 Project\2021-UoA-DATASCI-792-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E0E031-A629-478E-9712-D883497980C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB5B7C3-2615-46FE-8599-D1DEC133EAC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="3945" windowWidth="21600" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="2070" windowWidth="21600" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positional data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -84,9 +84,6 @@
     <t>16-23 - Replacement</t>
   </si>
   <si>
-    <t>Preferred position</t>
-  </si>
-  <si>
     <t>Abel, Robbie</t>
   </si>
   <si>
@@ -376,6 +373,12 @@
   </si>
   <si>
     <t>Fullback</t>
+  </si>
+  <si>
+    <t>Pref. pos (number)</t>
+  </si>
+  <si>
+    <t>Pref. pos (text)</t>
   </si>
 </sst>
 </file>
@@ -1225,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="T67" sqref="T67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,18 +1287,18 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1349,15 +1352,15 @@
         <v>2</v>
       </c>
       <c r="S2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -1411,15 +1414,15 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1473,15 +1476,15 @@
         <v>2</v>
       </c>
       <c r="S4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -1535,15 +1538,15 @@
         <v>7</v>
       </c>
       <c r="S5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1597,15 +1600,15 @@
         <v>14</v>
       </c>
       <c r="S6" t="s">
+        <v>103</v>
+      </c>
+      <c r="T6" t="s">
         <v>104</v>
-      </c>
-      <c r="T6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1659,15 +1662,15 @@
         <v>14</v>
       </c>
       <c r="S7" t="s">
+        <v>103</v>
+      </c>
+      <c r="T7" t="s">
         <v>104</v>
-      </c>
-      <c r="T7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1721,15 +1724,15 @@
         <v>8</v>
       </c>
       <c r="S8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1783,15 +1786,15 @@
         <v>5</v>
       </c>
       <c r="S9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1845,15 +1848,15 @@
         <v>5</v>
       </c>
       <c r="S10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1907,15 +1910,15 @@
         <v>8</v>
       </c>
       <c r="S11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1969,15 +1972,15 @@
         <v>12</v>
       </c>
       <c r="S12" t="s">
+        <v>109</v>
+      </c>
+      <c r="T12" t="s">
         <v>110</v>
-      </c>
-      <c r="T12" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2031,15 +2034,15 @@
         <v>5</v>
       </c>
       <c r="S13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2093,15 +2096,15 @@
         <v>3</v>
       </c>
       <c r="S14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -2155,15 +2158,15 @@
         <v>12</v>
       </c>
       <c r="S15" t="s">
+        <v>109</v>
+      </c>
+      <c r="T15" t="s">
         <v>110</v>
-      </c>
-      <c r="T15" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2217,15 +2220,15 @@
         <v>9</v>
       </c>
       <c r="S16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2279,15 +2282,15 @@
         <v>9</v>
       </c>
       <c r="S17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2341,15 +2344,15 @@
         <v>7</v>
       </c>
       <c r="S18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2403,15 +2406,15 @@
         <v>5</v>
       </c>
       <c r="S19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -2465,15 +2468,15 @@
         <v>10</v>
       </c>
       <c r="S20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -2527,15 +2530,15 @@
         <v>1</v>
       </c>
       <c r="S21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2589,15 +2592,15 @@
         <v>8</v>
       </c>
       <c r="S22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2651,15 +2654,15 @@
         <v>13</v>
       </c>
       <c r="S23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2713,15 +2716,15 @@
         <v>7</v>
       </c>
       <c r="S24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2775,15 +2778,15 @@
         <v>4</v>
       </c>
       <c r="S25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2837,15 +2840,15 @@
         <v>10</v>
       </c>
       <c r="S26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2899,15 +2902,15 @@
         <v>3</v>
       </c>
       <c r="S27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2961,15 +2964,15 @@
         <v>14</v>
       </c>
       <c r="S28" t="s">
+        <v>103</v>
+      </c>
+      <c r="T28" t="s">
         <v>104</v>
-      </c>
-      <c r="T28" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3023,15 +3026,15 @@
         <v>4</v>
       </c>
       <c r="S29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30">
         <v>6</v>
@@ -3085,15 +3088,15 @@
         <v>1</v>
       </c>
       <c r="S30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -3147,15 +3150,15 @@
         <v>2</v>
       </c>
       <c r="S31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -3209,15 +3212,15 @@
         <v>4</v>
       </c>
       <c r="S32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -3271,15 +3274,15 @@
         <v>10</v>
       </c>
       <c r="S33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -3333,15 +3336,15 @@
         <v>9</v>
       </c>
       <c r="S34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -3395,15 +3398,15 @@
         <v>1</v>
       </c>
       <c r="S35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -3457,15 +3460,15 @@
         <v>13</v>
       </c>
       <c r="S36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -3519,15 +3522,15 @@
         <v>14</v>
       </c>
       <c r="S37" t="s">
+        <v>103</v>
+      </c>
+      <c r="T37" t="s">
         <v>104</v>
-      </c>
-      <c r="T37" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -3581,15 +3584,15 @@
         <v>6</v>
       </c>
       <c r="S38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -3643,15 +3646,15 @@
         <v>1</v>
       </c>
       <c r="S39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -3705,15 +3708,15 @@
         <v>6</v>
       </c>
       <c r="S40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -3767,15 +3770,15 @@
         <v>6</v>
       </c>
       <c r="S41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -3829,15 +3832,15 @@
         <v>10</v>
       </c>
       <c r="S42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3891,15 +3894,15 @@
         <v>1</v>
       </c>
       <c r="S43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -3953,15 +3956,15 @@
         <v>11</v>
       </c>
       <c r="S44" t="s">
+        <v>103</v>
+      </c>
+      <c r="T44" t="s">
         <v>104</v>
-      </c>
-      <c r="T44" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -4015,15 +4018,15 @@
         <v>8</v>
       </c>
       <c r="S45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -4077,15 +4080,15 @@
         <v>3</v>
       </c>
       <c r="S46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -4139,15 +4142,15 @@
         <v>2</v>
       </c>
       <c r="S47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -4201,15 +4204,15 @@
         <v>9</v>
       </c>
       <c r="S48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4263,15 +4266,15 @@
         <v>2</v>
       </c>
       <c r="S49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -4325,15 +4328,15 @@
         <v>4</v>
       </c>
       <c r="S50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4387,15 +4390,15 @@
         <v>6</v>
       </c>
       <c r="S51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -4449,15 +4452,15 @@
         <v>2</v>
       </c>
       <c r="S52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -4511,15 +4514,15 @@
         <v>8</v>
       </c>
       <c r="S53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4573,15 +4576,15 @@
         <v>15</v>
       </c>
       <c r="S54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4635,15 +4638,15 @@
         <v>3</v>
       </c>
       <c r="S55" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -4697,15 +4700,15 @@
         <v>12</v>
       </c>
       <c r="S56" t="s">
+        <v>109</v>
+      </c>
+      <c r="T56" t="s">
         <v>110</v>
-      </c>
-      <c r="T56" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -4759,15 +4762,15 @@
         <v>13</v>
       </c>
       <c r="S57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4821,15 +4824,15 @@
         <v>15</v>
       </c>
       <c r="S58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -4883,15 +4886,15 @@
         <v>6</v>
       </c>
       <c r="S59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4945,15 +4948,15 @@
         <v>4</v>
       </c>
       <c r="S60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -5007,15 +5010,15 @@
         <v>8</v>
       </c>
       <c r="S61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -5069,15 +5072,15 @@
         <v>9</v>
       </c>
       <c r="S62" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -5131,15 +5134,15 @@
         <v>3</v>
       </c>
       <c r="S63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -5193,15 +5196,15 @@
         <v>15</v>
       </c>
       <c r="S64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -5255,15 +5258,15 @@
         <v>2</v>
       </c>
       <c r="S65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -5317,10 +5320,10 @@
         <v>5</v>
       </c>
       <c r="S66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
@@ -5376,77 +5379,80 @@
         <v>16</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>94</v>
+        <v>115</v>
+      </c>
+      <c r="T67" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H69" t="s">
+        <v>82</v>
+      </c>
+      <c r="L69" t="s">
         <v>83</v>
-      </c>
-      <c r="L69" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
+        <v>87</v>
+      </c>
+      <c r="P73" t="s">
         <v>88</v>
-      </c>
-      <c r="P73" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
+        <v>89</v>
+      </c>
+      <c r="G74" t="s">
+        <v>91</v>
+      </c>
+      <c r="P74" t="s">
         <v>90</v>
-      </c>
-      <c r="G74" t="s">
-        <v>92</v>
-      </c>
-      <c r="P74" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>